<commit_message>
Actualización total desde local
</commit_message>
<xml_diff>
--- a/Directorio_Afiliados_2025.xlsx
+++ b/Directorio_Afiliados_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6115d10aab34be5f/LinaM/Alsum/Comercial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Mauricio\Desktop\Analisis_Estrategico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{39522267-36FC-4806-BB78-5A6DD4A1ADB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B47EF8DD-59DA-4ECB-86BE-B89DE4156CC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCDACB36-C827-4939-96ED-9C75A9A6DCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4FC2C70F-FC4A-4210-8DA5-2DC061F51367}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FC2C70F-FC4A-4210-8DA5-2DC061F51367}"/>
   </bookViews>
   <sheets>
     <sheet name="Directorio 2025" sheetId="1" r:id="rId1"/>
@@ -76,20 +76,11 @@
     </comment>
     <comment ref="D59" authorId="1" shapeId="0" xr:uid="{426A0EC9-67E1-4963-A597-AF62A5928FA3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Intermediario de seguros
 Corredores de reaseguro</t>
-        </r>
       </text>
     </comment>
     <comment ref="AA91" authorId="2" shapeId="0" xr:uid="{610CDD1E-02A5-4E12-ADC2-64D61496BCBC}">
@@ -118,19 +109,10 @@
     </comment>
     <comment ref="A105" authorId="3" shapeId="0" xr:uid="{B0EE6CD7-C55F-4010-9AE0-0DBFFC500054}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Cambiar nombre</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -6679,16 +6661,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Poppins"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Poppins"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF212529"/>
       <name val="Poppins"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
@@ -8664,29 +8649,49 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.85546875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="108" customWidth="1"/>
-    <col min="2" max="3" width="16.85546875" style="19"/>
-    <col min="4" max="4" width="16.85546875" style="160"/>
-    <col min="5" max="8" width="16.85546875" style="19"/>
-    <col min="9" max="9" width="16.85546875" style="299"/>
-    <col min="10" max="11" width="0" style="299" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="0" style="300" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="0" style="289" hidden="1" customWidth="1"/>
-    <col min="15" max="16" width="16.85546875" style="19"/>
-    <col min="17" max="17" width="16.85546875" style="231"/>
-    <col min="18" max="19" width="16.85546875" style="19"/>
-    <col min="20" max="20" width="16.85546875" style="212"/>
-    <col min="21" max="22" width="16.85546875" style="19"/>
-    <col min="23" max="23" width="16.85546875" style="212"/>
-    <col min="24" max="16384" width="16.85546875" style="19"/>
+    <col min="1" max="1" width="73.88671875" style="108" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="171.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="160" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="59.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="299" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="299" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59.44140625" style="299" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" style="300" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" style="300" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.88671875" style="289" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.88671875" style="231" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.88671875" style="212" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="68.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5546875" style="212" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="121.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="63.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="114.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32" style="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="16.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="54.6" customHeight="1">
+    <row r="1" spans="1:35" ht="43.2">
       <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
@@ -8790,7 +8795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="36" customFormat="1" ht="29.1" customHeight="1">
+    <row r="2" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A2" s="121" t="s">
         <v>33</v>
       </c>
@@ -8877,7 +8882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="3" spans="1:35" s="36" customFormat="1">
       <c r="A3" s="121" t="s">
         <v>56</v>
       </c>
@@ -8972,7 +8977,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="36" customFormat="1" ht="33.6" customHeight="1">
+    <row r="4" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A4" s="121" t="s">
         <v>75</v>
       </c>
@@ -9059,7 +9064,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="36" customFormat="1" ht="27.95" customHeight="1">
+    <row r="5" spans="1:35" s="36" customFormat="1">
       <c r="A5" s="75" t="s">
         <v>87</v>
       </c>
@@ -9154,7 +9159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="6" spans="1:35" s="36" customFormat="1">
       <c r="A6" s="121" t="s">
         <v>107</v>
       </c>
@@ -9239,7 +9244,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="48" customFormat="1" ht="32.450000000000003" customHeight="1">
+    <row r="7" spans="1:35" s="48" customFormat="1">
       <c r="A7" s="77" t="s">
         <v>118</v>
       </c>
@@ -9328,7 +9333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="8" spans="1:35" s="36" customFormat="1">
       <c r="A8" s="75" t="s">
         <v>129</v>
       </c>
@@ -9409,7 +9414,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="9" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A9" s="75" t="s">
         <v>143</v>
       </c>
@@ -9496,7 +9501,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="10" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A10" s="121" t="s">
         <v>156</v>
       </c>
@@ -9593,7 +9598,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="11" spans="1:35" s="36" customFormat="1">
       <c r="A11" s="121" t="s">
         <v>174</v>
       </c>
@@ -9692,7 +9697,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="12" spans="1:35" s="36" customFormat="1">
       <c r="A12" s="121" t="s">
         <v>196</v>
       </c>
@@ -9781,7 +9786,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="13" spans="1:35" s="36" customFormat="1" ht="72">
       <c r="A13" s="121" t="s">
         <v>211</v>
       </c>
@@ -9866,7 +9871,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="14" spans="1:35" s="48" customFormat="1" ht="20.399999999999999">
       <c r="A14" s="121" t="s">
         <v>224</v>
       </c>
@@ -9943,7 +9948,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="15" spans="1:35" s="48" customFormat="1">
       <c r="A15" s="121" t="s">
         <v>234</v>
       </c>
@@ -10032,7 +10037,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="16" spans="1:35" s="36" customFormat="1">
       <c r="A16" s="121" t="s">
         <v>247</v>
       </c>
@@ -10127,7 +10132,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="17" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A17" s="75" t="s">
         <v>262</v>
       </c>
@@ -10198,7 +10203,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="18" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A18" s="121" t="s">
         <v>272</v>
       </c>
@@ -10285,7 +10290,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="19" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A19" s="121" t="s">
         <v>285</v>
       </c>
@@ -10384,7 +10389,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="20" spans="1:35" s="36" customFormat="1">
       <c r="A20" s="121" t="s">
         <v>305</v>
       </c>
@@ -10471,7 +10476,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="21" spans="1:35" s="36" customFormat="1">
       <c r="A21" s="121" t="s">
         <v>319</v>
       </c>
@@ -10564,7 +10569,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="22" spans="1:35" s="36" customFormat="1">
       <c r="A22" s="121" t="s">
         <v>335</v>
       </c>
@@ -10649,7 +10654,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="23" spans="1:35" s="48" customFormat="1">
       <c r="A23" s="75" t="s">
         <v>348</v>
       </c>
@@ -10724,7 +10729,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="24" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A24" s="105" t="s">
         <v>360</v>
       </c>
@@ -10801,7 +10806,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="25" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="25" spans="1:35" s="36" customFormat="1">
       <c r="A25" s="121" t="s">
         <v>373</v>
       </c>
@@ -10881,7 +10886,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="26" spans="1:35" s="36" customFormat="1">
       <c r="A26" s="75" t="s">
         <v>387</v>
       </c>
@@ -10947,7 +10952,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="27" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="27" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A27" s="75" t="s">
         <v>397</v>
       </c>
@@ -11021,7 +11026,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="28" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A28" s="121" t="s">
         <v>409</v>
       </c>
@@ -11113,7 +11118,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="29" spans="1:35" s="36" customFormat="1">
       <c r="A29" s="75" t="s">
         <v>428</v>
       </c>
@@ -11177,7 +11182,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="30" spans="1:35" s="36" customFormat="1">
       <c r="A30" s="144" t="s">
         <v>435</v>
       </c>
@@ -11265,7 +11270,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="31" spans="1:35" s="36" customFormat="1">
       <c r="A31" s="75" t="s">
         <v>453</v>
       </c>
@@ -11344,7 +11349,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="32" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="32" spans="1:35" s="36" customFormat="1">
       <c r="A32" s="75" t="s">
         <v>464</v>
       </c>
@@ -11423,7 +11428,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="33" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="33" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A33" s="75" t="s">
         <v>475</v>
       </c>
@@ -11489,7 +11494,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="34" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A34" s="121" t="s">
         <v>484</v>
       </c>
@@ -11581,7 +11586,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="35" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="35" spans="1:35" s="36" customFormat="1">
       <c r="A35" s="144" t="s">
         <v>498</v>
       </c>
@@ -11671,7 +11676,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="36" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="36" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A36" s="121" t="s">
         <v>514</v>
       </c>
@@ -11761,7 +11766,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="37" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="37" spans="1:35" s="36" customFormat="1">
       <c r="A37" s="75" t="s">
         <v>534</v>
       </c>
@@ -11844,7 +11849,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="38" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="38" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A38" s="75" t="s">
         <v>549</v>
       </c>
@@ -11931,7 +11936,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="39" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="39" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A39" s="75" t="s">
         <v>563</v>
       </c>
@@ -12011,7 +12016,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="40" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="40" spans="1:35" s="36" customFormat="1">
       <c r="A40" s="121" t="s">
         <v>574</v>
       </c>
@@ -12087,7 +12092,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="41" spans="1:35" s="36" customFormat="1">
       <c r="A41" s="121" t="s">
         <v>583</v>
       </c>
@@ -12171,7 +12176,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="42" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="42" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A42" s="75" t="s">
         <v>597</v>
       </c>
@@ -12248,7 +12253,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="43" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="43" spans="1:35" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A43" s="75" t="s">
         <v>608</v>
       </c>
@@ -12319,7 +12324,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="44" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="44" spans="1:35" s="48" customFormat="1">
       <c r="A44" s="75" t="s">
         <v>616</v>
       </c>
@@ -12396,7 +12401,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="45" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="45" spans="1:35" s="48" customFormat="1">
       <c r="A45" s="105" t="s">
         <v>627</v>
       </c>
@@ -12471,7 +12476,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="46" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="46" spans="1:35" s="48" customFormat="1">
       <c r="A46" s="105" t="s">
         <v>635</v>
       </c>
@@ -12543,7 +12548,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="47" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="47" spans="1:35" s="36" customFormat="1">
       <c r="A47" s="105" t="s">
         <v>647</v>
       </c>
@@ -12612,7 +12617,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="48" spans="1:35" s="36" customFormat="1" ht="26.45" customHeight="1">
+    <row r="48" spans="1:35" s="36" customFormat="1">
       <c r="A48" s="75" t="s">
         <v>657</v>
       </c>
@@ -12683,7 +12688,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="49" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="49" spans="1:35" s="36" customFormat="1">
       <c r="A49" s="105" t="s">
         <v>665</v>
       </c>
@@ -12750,7 +12755,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="50" spans="1:35" s="36" customFormat="1" ht="23.45" customHeight="1">
+    <row r="50" spans="1:35" s="36" customFormat="1" ht="43.2">
       <c r="A50" s="77" t="s">
         <v>675</v>
       </c>
@@ -12827,7 +12832,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="51" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="51" spans="1:35" s="48" customFormat="1">
       <c r="A51" s="77" t="s">
         <v>688</v>
       </c>
@@ -12896,7 +12901,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="52" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="52" spans="1:35" s="36" customFormat="1">
       <c r="A52" s="75" t="s">
         <v>697</v>
       </c>
@@ -12967,7 +12972,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="53" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="53" spans="1:35" s="48" customFormat="1">
       <c r="A53" s="109" t="s">
         <v>708</v>
       </c>
@@ -13039,7 +13044,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="54" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="54" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A54" s="75" t="s">
         <v>718</v>
       </c>
@@ -13113,7 +13118,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="55" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="55" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A55" s="121" t="s">
         <v>729</v>
       </c>
@@ -13202,7 +13207,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="56" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="56" spans="1:35" s="48" customFormat="1" ht="43.2">
       <c r="A56" s="121" t="s">
         <v>742</v>
       </c>
@@ -13287,7 +13292,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="57" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="57" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A57" s="121" t="s">
         <v>755</v>
       </c>
@@ -13377,7 +13382,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="58" spans="1:35" s="36" customFormat="1">
       <c r="A58" s="77" t="s">
         <v>769</v>
       </c>
@@ -13454,7 +13459,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="59" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="59" spans="1:35" s="36" customFormat="1" ht="43.2">
       <c r="A59" s="77" t="s">
         <v>778</v>
       </c>
@@ -13528,7 +13533,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="60" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="60" spans="1:35" s="36" customFormat="1">
       <c r="A60" s="121" t="s">
         <v>789</v>
       </c>
@@ -13606,7 +13611,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="61" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="61" spans="1:35" s="36" customFormat="1">
       <c r="A61" s="75" t="s">
         <v>799</v>
       </c>
@@ -13677,7 +13682,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="62" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="62" spans="1:35" s="36" customFormat="1" ht="28.8">
       <c r="A62" s="121" t="s">
         <v>810</v>
       </c>
@@ -13777,7 +13782,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="63" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="63" spans="1:35" s="36" customFormat="1">
       <c r="A63" s="75" t="s">
         <v>826</v>
       </c>
@@ -13852,7 +13857,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="64" spans="1:35" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="64" spans="1:35" s="36" customFormat="1">
       <c r="A64" s="121" t="s">
         <v>838</v>
       </c>
@@ -13944,7 +13949,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="65" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="65" spans="1:69" s="36" customFormat="1">
       <c r="A65" s="75" t="s">
         <v>856</v>
       </c>
@@ -14018,7 +14023,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="66" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="66" spans="1:69" s="48" customFormat="1">
       <c r="A66" s="75" t="s">
         <v>866</v>
       </c>
@@ -14089,7 +14094,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="67" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="67" spans="1:69" s="36" customFormat="1">
       <c r="A67" s="121" t="s">
         <v>877</v>
       </c>
@@ -14168,7 +14173,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="68" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="68" spans="1:69" s="36" customFormat="1">
       <c r="A68" s="75" t="s">
         <v>889</v>
       </c>
@@ -14240,7 +14245,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="69" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="69" spans="1:69" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A69" s="121" t="s">
         <v>898</v>
       </c>
@@ -14324,7 +14329,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="70" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="70" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A70" s="121" t="s">
         <v>911</v>
       </c>
@@ -14409,7 +14414,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="71" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="71" spans="1:69" s="36" customFormat="1">
       <c r="A71" s="161" t="s">
         <v>924</v>
       </c>
@@ -14483,7 +14488,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="72" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="72" spans="1:69" s="36" customFormat="1">
       <c r="A72" s="75" t="s">
         <v>936</v>
       </c>
@@ -14583,7 +14588,7 @@
       <c r="BP72" s="48"/>
       <c r="BQ72" s="48"/>
     </row>
-    <row r="73" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="73" spans="1:69" s="36" customFormat="1">
       <c r="A73" s="121" t="s">
         <v>945</v>
       </c>
@@ -14677,7 +14682,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="74" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="74" spans="1:69" s="36" customFormat="1">
       <c r="A74" s="75" t="s">
         <v>964</v>
       </c>
@@ -14752,7 +14757,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="75" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="75" spans="1:69" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A75" s="162" t="s">
         <v>975</v>
       </c>
@@ -14836,7 +14841,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="76" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="76" spans="1:69" s="36" customFormat="1">
       <c r="A76" s="121" t="s">
         <v>989</v>
       </c>
@@ -14922,7 +14927,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="77" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="77" spans="1:69" s="48" customFormat="1">
       <c r="A77" s="121" t="s">
         <v>998</v>
       </c>
@@ -15003,7 +15008,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="78" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="78" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A78" s="75" t="s">
         <v>1008</v>
       </c>
@@ -15068,7 +15073,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="79" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="79" spans="1:69" s="36" customFormat="1">
       <c r="A79" s="109" t="s">
         <v>1014</v>
       </c>
@@ -15142,7 +15147,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="80" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="80" spans="1:69" s="36" customFormat="1">
       <c r="A80" s="75" t="s">
         <v>1028</v>
       </c>
@@ -15224,7 +15229,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="81" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="81" spans="1:69" s="36" customFormat="1">
       <c r="A81" s="105" t="s">
         <v>1042</v>
       </c>
@@ -15301,7 +15306,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="82" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="82" spans="1:69" s="48" customFormat="1">
       <c r="A82" s="121" t="s">
         <v>1054</v>
       </c>
@@ -15430,7 +15435,7 @@
       <c r="BP82" s="36"/>
       <c r="BQ82" s="36"/>
     </row>
-    <row r="83" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="83" spans="1:69" s="48" customFormat="1">
       <c r="A83" s="121" t="s">
         <v>1071</v>
       </c>
@@ -15507,7 +15512,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="84" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="84" spans="1:69" s="48" customFormat="1">
       <c r="A84" s="75" t="s">
         <v>1083</v>
       </c>
@@ -15570,7 +15575,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="85" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="85" spans="1:69" s="36" customFormat="1">
       <c r="A85" s="75" t="s">
         <v>1090</v>
       </c>
@@ -15679,7 +15684,7 @@
       <c r="BP85" s="48"/>
       <c r="BQ85" s="48"/>
     </row>
-    <row r="86" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="86" spans="1:69" s="36" customFormat="1">
       <c r="A86" s="121" t="s">
         <v>1100</v>
       </c>
@@ -15776,7 +15781,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="87" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="87" spans="1:69" s="36" customFormat="1">
       <c r="A87" s="75" t="s">
         <v>1116</v>
       </c>
@@ -15854,7 +15859,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="88" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="88" spans="1:69" s="36" customFormat="1" ht="72">
       <c r="A88" s="75" t="s">
         <v>1128</v>
       </c>
@@ -15928,7 +15933,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="89" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="89" spans="1:69" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A89" s="170" t="s">
         <v>1137</v>
       </c>
@@ -16012,7 +16017,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="90" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="90" spans="1:69" s="36" customFormat="1">
       <c r="A90" s="121" t="s">
         <v>1147</v>
       </c>
@@ -16090,7 +16095,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="91" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="91" spans="1:69" s="36" customFormat="1">
       <c r="A91" s="121" t="s">
         <v>1159</v>
       </c>
@@ -16178,7 +16183,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="92" spans="1:69" s="36" customFormat="1" ht="38.450000000000003" customHeight="1">
+    <row r="92" spans="1:69" s="36" customFormat="1">
       <c r="A92" s="105" t="s">
         <v>1179</v>
       </c>
@@ -16256,7 +16261,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="93" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="93" spans="1:69" s="48" customFormat="1">
       <c r="A93" s="121" t="s">
         <v>1191</v>
       </c>
@@ -16339,7 +16344,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="94" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="94" spans="1:69" s="36" customFormat="1">
       <c r="A94" s="77" t="s">
         <v>1203</v>
       </c>
@@ -16439,7 +16444,7 @@
       <c r="BP94" s="48"/>
       <c r="BQ94" s="48"/>
     </row>
-    <row r="95" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="95" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A95" s="121" t="s">
         <v>1211</v>
       </c>
@@ -16532,7 +16537,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="96" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="96" spans="1:69" s="36" customFormat="1">
       <c r="A96" s="121" t="s">
         <v>1229</v>
       </c>
@@ -16621,7 +16626,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="97" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="97" spans="1:69" s="36" customFormat="1">
       <c r="A97" s="121" t="s">
         <v>1244</v>
       </c>
@@ -16707,7 +16712,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="98" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="98" spans="1:69" s="36" customFormat="1">
       <c r="A98" s="75" t="s">
         <v>1259</v>
       </c>
@@ -16776,7 +16781,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="99" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="99" spans="1:69" s="36" customFormat="1">
       <c r="A99" s="75" t="s">
         <v>1269</v>
       </c>
@@ -16851,7 +16856,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="100" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="100" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A100" s="75" t="s">
         <v>1278</v>
       </c>
@@ -16916,7 +16921,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="101" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="101" spans="1:69" s="36" customFormat="1">
       <c r="A101" s="144" t="s">
         <v>1286</v>
       </c>
@@ -17009,7 +17014,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="102" spans="1:69" s="36" customFormat="1" ht="28.5" customHeight="1">
+    <row r="102" spans="1:69" s="36" customFormat="1">
       <c r="A102" s="121" t="s">
         <v>1299</v>
       </c>
@@ -17087,7 +17092,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="103" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="103" spans="1:69" s="36" customFormat="1">
       <c r="A103" s="75" t="s">
         <v>1307</v>
       </c>
@@ -17149,7 +17154,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="104" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="104" spans="1:69" s="36" customFormat="1">
       <c r="A104" s="75" t="s">
         <v>1312</v>
       </c>
@@ -17227,7 +17232,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="105" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="105" spans="1:69" s="36" customFormat="1">
       <c r="A105" s="109" t="s">
         <v>1323</v>
       </c>
@@ -17302,7 +17307,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="106" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="106" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A106" s="75" t="s">
         <v>1337</v>
       </c>
@@ -17385,7 +17390,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="107" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="107" spans="1:69" s="48" customFormat="1">
       <c r="A107" s="75" t="s">
         <v>1349</v>
       </c>
@@ -17496,7 +17501,7 @@
       <c r="BP107" s="36"/>
       <c r="BQ107" s="36"/>
     </row>
-    <row r="108" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="108" spans="1:69" s="48" customFormat="1">
       <c r="A108" s="75" t="s">
         <v>1360</v>
       </c>
@@ -17575,7 +17580,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="109" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="109" spans="1:69" s="36" customFormat="1" ht="20.399999999999999">
       <c r="A109" s="121" t="s">
         <v>1371</v>
       </c>
@@ -17703,7 +17708,7 @@
       <c r="BP109" s="48"/>
       <c r="BQ109" s="48"/>
     </row>
-    <row r="110" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="110" spans="1:69" s="36" customFormat="1">
       <c r="A110" s="77" t="s">
         <v>1387</v>
       </c>
@@ -17818,7 +17823,7 @@
       <c r="BP110" s="48"/>
       <c r="BQ110" s="48"/>
     </row>
-    <row r="111" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="111" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A111" s="75" t="s">
         <v>1401</v>
       </c>
@@ -17893,7 +17898,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="112" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="112" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A112" s="121" t="s">
         <v>1412</v>
       </c>
@@ -17982,7 +17987,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="113" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="113" spans="1:69" s="36" customFormat="1">
       <c r="A113" s="75" t="s">
         <v>1428</v>
       </c>
@@ -18056,7 +18061,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="114" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="114" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A114" s="75" t="s">
         <v>1440</v>
       </c>
@@ -18129,7 +18134,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="115" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="115" spans="1:69" s="36" customFormat="1" ht="43.2">
       <c r="A115" s="75" t="s">
         <v>1450</v>
       </c>
@@ -18209,7 +18214,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="116" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="116" spans="1:69" s="36" customFormat="1">
       <c r="A116" s="75" t="s">
         <v>1464</v>
       </c>
@@ -18294,7 +18299,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="117" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="117" spans="1:69" s="48" customFormat="1">
       <c r="A117" s="75" t="s">
         <v>1476</v>
       </c>
@@ -18419,7 +18424,7 @@
       <c r="BP117" s="36"/>
       <c r="BQ117" s="36"/>
     </row>
-    <row r="118" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="118" spans="1:69" s="36" customFormat="1">
       <c r="A118" s="121" t="s">
         <v>1491</v>
       </c>
@@ -18509,7 +18514,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="119" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="119" spans="1:69" s="36" customFormat="1">
       <c r="A119" s="144" t="s">
         <v>1506</v>
       </c>
@@ -18596,7 +18601,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="120" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="120" spans="1:69" s="48" customFormat="1">
       <c r="A120" s="121" t="s">
         <v>1518</v>
       </c>
@@ -18687,7 +18692,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="121" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="121" spans="1:69" s="36" customFormat="1">
       <c r="A121" s="121" t="s">
         <v>1535</v>
       </c>
@@ -18803,7 +18808,7 @@
       <c r="BP121" s="48"/>
       <c r="BQ121" s="48"/>
     </row>
-    <row r="122" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="122" spans="1:69" s="36" customFormat="1">
       <c r="A122" s="121" t="s">
         <v>1549</v>
       </c>
@@ -18890,7 +18895,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="123" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="123" spans="1:69" s="48" customFormat="1">
       <c r="A123" s="75" t="s">
         <v>1562</v>
       </c>
@@ -18994,7 +18999,7 @@
       <c r="BP123" s="36"/>
       <c r="BQ123" s="36"/>
     </row>
-    <row r="124" spans="1:69" s="42" customFormat="1" ht="22.5" customHeight="1">
+    <row r="124" spans="1:69" s="42" customFormat="1" ht="86.4">
       <c r="A124" s="75" t="s">
         <v>1571</v>
       </c>
@@ -19091,7 +19096,7 @@
       <c r="BP124" s="48"/>
       <c r="BQ124" s="48"/>
     </row>
-    <row r="125" spans="1:69" s="42" customFormat="1" ht="22.5" customHeight="1">
+    <row r="125" spans="1:69" s="42" customFormat="1" ht="28.8">
       <c r="A125" s="75" t="s">
         <v>1580</v>
       </c>
@@ -19196,7 +19201,7 @@
       <c r="BP125" s="36"/>
       <c r="BQ125" s="36"/>
     </row>
-    <row r="126" spans="1:69" s="29" customFormat="1" ht="22.5" customHeight="1">
+    <row r="126" spans="1:69" s="29" customFormat="1">
       <c r="A126" s="121" t="s">
         <v>1590</v>
       </c>
@@ -19319,7 +19324,7 @@
       <c r="BP126" s="48"/>
       <c r="BQ126" s="48"/>
     </row>
-    <row r="127" spans="1:69" s="29" customFormat="1" ht="22.5" customHeight="1">
+    <row r="127" spans="1:69" s="29" customFormat="1" ht="28.8">
       <c r="A127" s="121" t="s">
         <v>1603</v>
       </c>
@@ -19447,7 +19452,7 @@
       <c r="BP127" s="48"/>
       <c r="BQ127" s="48"/>
     </row>
-    <row r="128" spans="1:69" s="29" customFormat="1" ht="22.5" customHeight="1">
+    <row r="128" spans="1:69" s="29" customFormat="1" ht="28.8">
       <c r="A128" s="75" t="s">
         <v>1623</v>
       </c>
@@ -19550,7 +19555,7 @@
       <c r="BP128" s="48"/>
       <c r="BQ128" s="48"/>
     </row>
-    <row r="129" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="129" spans="1:69" s="48" customFormat="1" ht="28.8">
       <c r="A129" s="121" t="s">
         <v>1632</v>
       </c>
@@ -19632,7 +19637,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="130" spans="1:69" s="48" customFormat="1" ht="29.25" customHeight="1">
+    <row r="130" spans="1:69" s="48" customFormat="1">
       <c r="A130" s="75" t="s">
         <v>1646</v>
       </c>
@@ -19740,7 +19745,7 @@
       <c r="BP130" s="36"/>
       <c r="BQ130" s="36"/>
     </row>
-    <row r="131" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="131" spans="1:69" s="36" customFormat="1">
       <c r="A131" s="75" t="s">
         <v>1657</v>
       </c>
@@ -19804,7 +19809,7 @@
       </c>
       <c r="AF131" s="48"/>
     </row>
-    <row r="132" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="132" spans="1:69" s="36" customFormat="1">
       <c r="A132" s="144" t="s">
         <v>1666</v>
       </c>
@@ -19921,7 +19926,7 @@
       <c r="BP132" s="48"/>
       <c r="BQ132" s="48"/>
     </row>
-    <row r="133" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="133" spans="1:69" s="36" customFormat="1">
       <c r="A133" s="77" t="s">
         <v>1674</v>
       </c>
@@ -20029,7 +20034,7 @@
       <c r="BP133" s="48"/>
       <c r="BQ133" s="48"/>
     </row>
-    <row r="134" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="134" spans="1:69" s="36" customFormat="1">
       <c r="A134" s="121" t="s">
         <v>1686</v>
       </c>
@@ -20116,7 +20121,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="135" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="135" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A135" s="75" t="s">
         <v>1701</v>
       </c>
@@ -20183,7 +20188,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="136" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="136" spans="1:69" s="36" customFormat="1">
       <c r="A136" s="75" t="s">
         <v>1711</v>
       </c>
@@ -20264,7 +20269,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="137" spans="1:69" s="36" customFormat="1" ht="22.5" customHeight="1">
+    <row r="137" spans="1:69" s="36" customFormat="1" ht="28.8">
       <c r="A137" s="75" t="s">
         <v>1723</v>
       </c>
@@ -20326,7 +20331,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="138" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="138" spans="1:69" s="48" customFormat="1">
       <c r="A138" s="173" t="s">
         <v>1730</v>
       </c>
@@ -20446,7 +20451,7 @@
       <c r="BP138" s="36"/>
       <c r="BQ138" s="36"/>
     </row>
-    <row r="139" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="139" spans="1:69" s="48" customFormat="1" ht="28.8">
       <c r="A139" s="121" t="s">
         <v>1741</v>
       </c>
@@ -20559,7 +20564,7 @@
       <c r="BP139" s="36"/>
       <c r="BQ139" s="36"/>
     </row>
-    <row r="140" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="140" spans="1:69" s="48" customFormat="1">
       <c r="A140" s="75" t="s">
         <v>1753</v>
       </c>
@@ -20668,7 +20673,7 @@
       <c r="BP140" s="36"/>
       <c r="BQ140" s="36"/>
     </row>
-    <row r="141" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="141" spans="1:69" s="48" customFormat="1">
       <c r="A141" s="77" t="s">
         <v>1764</v>
       </c>
@@ -20766,7 +20771,7 @@
       <c r="BP141" s="36"/>
       <c r="BQ141" s="36"/>
     </row>
-    <row r="142" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="142" spans="1:69" s="48" customFormat="1">
       <c r="A142" s="75" t="s">
         <v>1770</v>
       </c>
@@ -20824,7 +20829,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="143" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="143" spans="1:69" s="48" customFormat="1" ht="28.8">
       <c r="A143" s="75" t="s">
         <v>1776</v>
       </c>
@@ -20892,7 +20897,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="144" spans="1:69" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="144" spans="1:69" s="48" customFormat="1">
       <c r="A144" s="121" t="s">
         <v>1786</v>
       </c>
@@ -20988,7 +20993,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="145" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="145" spans="1:35" s="48" customFormat="1" ht="43.2">
       <c r="A145" s="77" t="s">
         <v>1803</v>
       </c>
@@ -21067,7 +21072,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="146" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="146" spans="1:35" s="48" customFormat="1">
       <c r="A146" s="121" t="s">
         <v>1814</v>
       </c>
@@ -21163,7 +21168,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="147" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="147" spans="1:35" s="48" customFormat="1" ht="20.399999999999999">
       <c r="A147" s="77" t="s">
         <v>1830</v>
       </c>
@@ -21222,7 +21227,7 @@
         <v>1836</v>
       </c>
     </row>
-    <row r="148" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="148" spans="1:35" s="48" customFormat="1">
       <c r="A148" s="75" t="s">
         <v>1837</v>
       </c>
@@ -21291,7 +21296,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="149" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="149" spans="1:35" s="48" customFormat="1">
       <c r="A149" s="75" t="s">
         <v>1850</v>
       </c>
@@ -21360,7 +21365,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="150" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="150" spans="1:35" s="48" customFormat="1">
       <c r="A150" s="106" t="s">
         <v>1860</v>
       </c>
@@ -21437,7 +21442,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="151" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="151" spans="1:35" s="48" customFormat="1" ht="43.2">
       <c r="A151" s="75" t="s">
         <v>1870</v>
       </c>
@@ -21510,7 +21515,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="152" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="152" spans="1:35" s="48" customFormat="1" ht="43.2">
       <c r="A152" s="75" t="s">
         <v>1881</v>
       </c>
@@ -21579,7 +21584,7 @@
       </c>
       <c r="AE152" s="36"/>
     </row>
-    <row r="153" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="153" spans="1:35" s="48" customFormat="1" ht="20.399999999999999">
       <c r="A153" s="105" t="s">
         <v>1892</v>
       </c>
@@ -21645,7 +21650,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="154" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="154" spans="1:35" s="48" customFormat="1" ht="20.399999999999999">
       <c r="A154" s="121" t="s">
         <v>1902</v>
       </c>
@@ -21735,7 +21740,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="155" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="155" spans="1:35" s="48" customFormat="1">
       <c r="A155" s="75" t="s">
         <v>1919</v>
       </c>
@@ -21804,7 +21809,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="156" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="156" spans="1:35" s="48" customFormat="1">
       <c r="A156" s="75" t="s">
         <v>1927</v>
       </c>
@@ -21869,7 +21874,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="157" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="157" spans="1:35" s="48" customFormat="1">
       <c r="A157" s="121" t="s">
         <v>1937</v>
       </c>
@@ -21955,7 +21960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="158" spans="1:35" s="48" customFormat="1" ht="22.5" customHeight="1">
+    <row r="158" spans="1:35" s="48" customFormat="1" ht="28.8">
       <c r="A158" s="75" t="s">
         <v>1947</v>
       </c>
@@ -22028,7 +22033,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="159" spans="1:35" s="48" customFormat="1" ht="24.6" customHeight="1">
+    <row r="159" spans="1:35" s="48" customFormat="1" ht="28.8">
       <c r="A159" s="107" t="s">
         <v>1956</v>
       </c>
@@ -22107,7 +22112,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="160" spans="1:35" s="88" customFormat="1" ht="15" customHeight="1">
+    <row r="160" spans="1:35" s="88" customFormat="1">
       <c r="A160" s="176" t="s">
         <v>1965</v>
       </c>
@@ -22173,7 +22178,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="161" spans="1:35" s="88" customFormat="1" ht="22.5" customHeight="1">
+    <row r="161" spans="1:35" s="88" customFormat="1">
       <c r="A161" s="106" t="s">
         <v>1974</v>
       </c>
@@ -22238,7 +22243,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="194" spans="16:16" ht="12.75" customHeight="1">
+    <row r="194" spans="16:16">
       <c r="P194" s="51" t="s">
         <v>1020</v>
       </c>
@@ -22601,11 +22606,11 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="5" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38.109375" customWidth="1"/>
+    <col min="3" max="5" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -22821,7 +22826,7 @@
         <v>45778</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="22.5">
+    <row r="12" spans="1:9">
       <c r="A12" s="90" t="s">
         <v>1996</v>
       </c>
@@ -23059,7 +23064,7 @@
         <v>45884</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="22.5">
+    <row r="26" spans="1:5">
       <c r="A26" s="90" t="s">
         <v>2008</v>
       </c>
@@ -23144,7 +23149,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="22.5">
+    <row r="31" spans="1:5">
       <c r="A31" s="90" t="s">
         <v>118</v>
       </c>
@@ -23254,20 +23259,20 @@
       <selection activeCell="F5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="19" customFormat="1" ht="12.75">
+    <row r="1" spans="1:49" s="19" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -23299,7 +23304,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="19" customFormat="1" ht="29.45" customHeight="1">
+    <row r="2" spans="1:49" s="19" customFormat="1" ht="29.4" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>2016</v>
       </c>
@@ -23494,19 +23499,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5">
+    <row r="1" spans="1:2" ht="19.8">
       <c r="A1" s="324" t="s">
         <v>2046</v>
       </c>
       <c r="B1" s="324"/>
     </row>
-    <row r="2" spans="1:2" ht="19.5">
+    <row r="2" spans="1:2" ht="19.8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -23514,7 +23519,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5">
+    <row r="3" spans="1:2" ht="19.8">
       <c r="A3" s="2" t="s">
         <v>2048</v>
       </c>
@@ -23522,7 +23527,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5">
+    <row r="4" spans="1:2" ht="19.8">
       <c r="A4" s="5" t="s">
         <v>2049</v>
       </c>
@@ -23530,7 +23535,7 @@
         <v>45330</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5">
+    <row r="5" spans="1:2" ht="19.8">
       <c r="A5" s="5" t="s">
         <v>2050</v>
       </c>
@@ -23538,7 +23543,7 @@
         <v>45339</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5">
+    <row r="6" spans="1:2" ht="19.8">
       <c r="A6" s="5" t="s">
         <v>2051</v>
       </c>
@@ -23546,7 +23551,7 @@
         <v>45342</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.5">
+    <row r="7" spans="1:2" ht="19.8">
       <c r="A7" s="7" t="s">
         <v>1919</v>
       </c>
@@ -23554,7 +23559,7 @@
         <v>45365</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5">
+    <row r="8" spans="1:2" ht="19.8">
       <c r="A8" s="7" t="s">
         <v>1259</v>
       </c>
@@ -23562,7 +23567,7 @@
         <v>45385</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19.5">
+    <row r="9" spans="1:2" ht="19.8">
       <c r="A9" s="2" t="s">
         <v>2052</v>
       </c>
@@ -23570,7 +23575,7 @@
         <v>45422</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="19.5">
+    <row r="10" spans="1:2" ht="19.8">
       <c r="A10" s="2" t="s">
         <v>2053</v>
       </c>
@@ -23578,7 +23583,7 @@
         <v>45433</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="19.5">
+    <row r="11" spans="1:2" ht="19.8">
       <c r="A11" s="2" t="s">
         <v>563</v>
       </c>
@@ -23586,7 +23591,7 @@
         <v>45443</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="19.5">
+    <row r="12" spans="1:2" ht="19.8">
       <c r="A12" s="2" t="s">
         <v>2054</v>
       </c>
@@ -23594,7 +23599,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="19.5">
+    <row r="13" spans="1:2" ht="19.8">
       <c r="A13" s="2" t="s">
         <v>1753</v>
       </c>
@@ -23602,7 +23607,7 @@
         <v>45460</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19.5">
+    <row r="14" spans="1:2" ht="19.8">
       <c r="A14" s="2" t="s">
         <v>2055</v>
       </c>
@@ -23610,7 +23615,7 @@
         <v>45496</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="19.5">
+    <row r="15" spans="1:2" ht="19.8">
       <c r="A15" s="2" t="s">
         <v>2056</v>
       </c>
@@ -23618,7 +23623,7 @@
         <v>45498</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="19.5">
+    <row r="16" spans="1:2" ht="19.8">
       <c r="A16" s="8" t="s">
         <v>2057</v>
       </c>
@@ -23626,7 +23631,7 @@
         <v>45503</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="19.5">
+    <row r="17" spans="1:2" ht="19.8">
       <c r="A17" s="2" t="s">
         <v>2058</v>
       </c>
@@ -23634,7 +23639,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="19.5">
+    <row r="18" spans="1:2" ht="19.8">
       <c r="A18" s="2" t="s">
         <v>2060</v>
       </c>
@@ -23642,7 +23647,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="19.5">
+    <row r="19" spans="1:2" ht="19.8">
       <c r="A19" s="2" t="s">
         <v>2062</v>
       </c>
@@ -23650,7 +23655,7 @@
         <v>45517</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="19.5">
+    <row r="20" spans="1:2" ht="19.8">
       <c r="A20" s="2" t="s">
         <v>2063</v>
       </c>
@@ -23658,7 +23663,7 @@
         <v>45537</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="19.5">
+    <row r="21" spans="1:2" ht="19.8">
       <c r="A21" s="2" t="s">
         <v>2064</v>
       </c>
@@ -23666,7 +23671,7 @@
         <v>45539</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="19.5">
+    <row r="22" spans="1:2" ht="19.8">
       <c r="A22" s="2" t="s">
         <v>2065</v>
       </c>
@@ -23674,7 +23679,7 @@
         <v>45545</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="19.5">
+    <row r="23" spans="1:2" ht="19.8">
       <c r="A23" s="2" t="s">
         <v>2066</v>
       </c>
@@ -23682,7 +23687,7 @@
         <v>45553</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="19.5">
+    <row r="24" spans="1:2" ht="19.8">
       <c r="A24" s="2" t="s">
         <v>2067</v>
       </c>
@@ -23690,7 +23695,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="19.5">
+    <row r="25" spans="1:2" ht="19.8">
       <c r="A25" s="5" t="s">
         <v>2068</v>
       </c>
@@ -23698,7 +23703,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="19.5">
+    <row r="26" spans="1:2" ht="19.8">
       <c r="A26" s="4" t="s">
         <v>2069</v>
       </c>

</xml_diff>